<commit_message>
casi termino con el procesamiento de las planillas de google forms, problemas para crear nuevo estudiante con model.estudiante.crear
</commit_message>
<xml_diff>
--- a/otherfiles/PlanillaMarwan.xlsx
+++ b/otherfiles/PlanillaMarwan.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Git\Orcaestra Finanzas\otherfiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{780C757E-FDC9-4B37-AF7B-9B86063BB63C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="585" windowWidth="21015" windowHeight="9345"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -82,9 +88,6 @@
     <t>Makarem Abdel</t>
   </si>
   <si>
-    <t>Kinder Música</t>
-  </si>
-  <si>
     <t>sdf</t>
   </si>
   <si>
@@ -131,12 +134,15 @@
   </si>
   <si>
     <t>=T3=H2&amp;", "&amp;G2&amp;"/"&amp;K2&amp;", "&amp;J2&amp;"/"&amp;N2&amp;", "&amp;M2</t>
+  </si>
+  <si>
+    <t>Kinder Musical</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
@@ -315,23 +321,94 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="FFFFFF"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="3C3C3C"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -366,7 +443,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -399,9 +476,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -434,6 +528,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -609,18 +720,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AA102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U2" sqref="U2"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
@@ -695,25 +806,25 @@
         <v>19</v>
       </c>
       <c r="U1" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="V1" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="W1" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="21" t="s">
+      <c r="X1" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="21" t="s">
+      <c r="Y1" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="21" t="s">
+      <c r="Z1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="21" t="s">
+      <c r="AA1" s="21" t="s">
         <v>33</v>
-      </c>
-      <c r="AA1" s="21" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -732,34 +843,34 @@
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="I2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="K2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="13" t="s">
         <v>22</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>23</v>
       </c>
       <c r="Q2" s="14">
         <v>43271</v>
@@ -771,14 +882,14 @@
         <v>234</v>
       </c>
       <c r="T2" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U2" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="V2" s="15" t="str">
         <f>I2&amp;"/"&amp;L2&amp;"/"&amp;O2</f>
-        <v>Kinder Música/N/A/N/A</v>
+        <v>Kinder Musical/N/A/N/A</v>
       </c>
       <c r="W2" s="15"/>
       <c r="X2" s="15"/>

</xml_diff>